<commit_message>
update code with real time data
</commit_message>
<xml_diff>
--- a/data/Dataset_v4.xlsx
+++ b/data/Dataset_v4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woojinheo/Desktop/github/travel_optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A796E36A-795F-A242-9DE6-F5C93C85EF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B4AF8F-F5FF-6044-8988-38E2D6C10F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5600" yWindow="680" windowWidth="22400" windowHeight="16480" xr2:uid="{4793D832-98B4-9B4B-B319-BFD6E3C3A9EB}"/>
   </bookViews>
@@ -2131,7 +2131,7 @@
   <dimension ref="A1:M139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>